<commit_message>
Update data with Grok-verified corrections
ATS Market Share (verified via xAI Grok):
- Workday: 7-8% → 12-14% (was underestimated)
- Bullhorn: 2-3% → 1-1.5% (was overstated)
- Total coverage: ~51% → ~56%

Job API Rate Limits (corrected):
- USAJobs: 10,000 rows → 100 rows/page with pagination
- Adzuna: 25 req/min → 100 req/day free tier

Updated files:
- app/services/ats_checker.py
- app/services/job_fetcher.py
- business_plan/MatchForge_Analysis_Verified.xlsx
- business_plan/MatchForge_Business_Plan_Verified.docx

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/business_plan/MatchForge_Analysis_Verified.xlsx
+++ b/business_plan/MatchForge_Analysis_Verified.xlsx
@@ -1078,6 +1078,7 @@
         </is>
       </c>
     </row>
+    <row r="3"/>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
@@ -1179,7 +1180,7 @@
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>~7-8%</t>
+          <t>12-14%</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -1368,7 +1369,7 @@
       </c>
       <c r="C15" s="4" t="inlineStr">
         <is>
-          <t>~2-3%</t>
+          <t>1-1.5%</t>
         </is>
       </c>
       <c r="D15" s="4" t="inlineStr">
@@ -1391,12 +1392,13 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>~51%</t>
+          <t>~56%</t>
         </is>
       </c>
       <c r="D16" s="13" t="n"/>
       <c r="E16" s="13" t="n"/>
     </row>
+    <row r="17"/>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
@@ -1576,6 +1578,8 @@
         </is>
       </c>
     </row>
+    <row r="29"/>
+    <row r="30"/>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Add ATS history to business plan (Grok-verified)
35+ years of ATS adoption history:
- 1990: First commercial ATS (Resumix)
- 1999: Taleo founded
- 2002: 50%+ large companies using ATS
- Today: 99% of Fortune 500 use ATS

Sources: SHRM, Harvard Business Review, Oracle, Indeed

Added to:
- business_plan/MatchForge_Business_Plan_Verified.docx
- business_plan/MatchForge_Analysis_Verified.xlsx (new sheet)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/business_plan/MatchForge_Analysis_Verified.xlsx
+++ b/business_plan/MatchForge_Analysis_Verified.xlsx
@@ -13,6 +13,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Privacy Infrastructure" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Competitor Pricing" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Costs Summary" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ATS History" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1078,7 +1079,6 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
@@ -1398,7 +1398,6 @@
       <c r="D16" s="13" t="n"/>
       <c r="E16" s="13" t="n"/>
     </row>
-    <row r="17"/>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
@@ -1578,8 +1577,6 @@
         </is>
       </c>
     </row>
-    <row r="29"/>
-    <row r="30"/>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
@@ -2565,4 +2562,163 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ATS ADOPTION HISTORY (Grok-verified)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Era</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Milestone</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Late 1970s-80s</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Early HR databases on mainframes (IBM)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SHRM</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>First commercial ATS - Resumix founded</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Harvard Business Review</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1999</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Taleo founded (web-based ATS)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Oracle</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2002</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>50%+ of large US companies using ATS</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SHRM</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2010s</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AI-driven screening, mobile integration</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Industry reports</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Today</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>99% of Fortune 500 use ATS</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Indeed Career Guide</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>KEY INSIGHT</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ATS has been filtering resumes for 35+ years. MatchForge checks against 10 systems (~56% market).</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add competitor analysis and clarify differentiation
ATS Resume Tool Competitors (Grok-verified):
- Jobscan: $49.95/mo - market leader
- SkillSyncer: $19.99-39.99/mo
- Resume Worded: $8/mo
- Enhancv: ~$14/mo
- ResyMatch.io: $8/mo

Honest Assessment:
- ATS checking alone is NOT unique (competitors do this)
- MatchForge differentiates via COMBINATION:
  • ATS optimization (table stakes)
  • Transparent 6-factor matching (unique)
  • Human coaching at subscription prices (unique)
  • Outcome tracking / feedback loop (unique)

Updated:
- business_plan/MatchForge_Business_Plan_Verified.docx
- business_plan/MatchForge_Analysis_Verified.xlsx (new sheet)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/business_plan/MatchForge_Analysis_Verified.xlsx
+++ b/business_plan/MatchForge_Analysis_Verified.xlsx
@@ -14,6 +14,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Competitor Pricing" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Costs Summary" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ATS History" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ATS Competitors" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2721,4 +2722,359 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ATS RESUME TOOL COMPETITORS (Grok-verified Jan 2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Tool</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Free Tier</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Paid Monthly</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Key Feature</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Jobscan</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Limited scans</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>$49.95/mo</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Market leader, job matching</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SkillSyncer</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Limited</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$19.99-39.99/mo</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>AI auto-optimization</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Resume Worded</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Basic checks</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$8/mo</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>25+ criteria checks</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Enhancv</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Basic builder</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>~$14/mo</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Resume builder + ATS</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ResyMatch.io</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Limited</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$8/mo</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Free tier from Cultivated Culture</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>MatchForge</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Full demo</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$9-29/mo (target)</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ATS + Matching + Coaching</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MATCHFORGE TRUE DIFFERENTIATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Jobscan</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>SkillSyncer</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>MatchForge</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ATS checking</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Transparent 6-factor matching</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Human coaching</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Outcome tracking</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Feedback loop validation</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Full stack (ATS+Match+Coach)</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>HONEST ASSESSMENT</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>ATS checking alone is NOT unique. The COMBINATION is the differentiator.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add LLM-powered match explanation feature
- New llm_explainer.py service supporting OpenAI, Anthropic, and xAI providers
- POST /api/v1/jobs/explain-match endpoint for AI explanations
- Demo script to test LLM integration
- AI implementation spec in docs/
- Updated business plan with AI roadmap
- Added openai and anthropic to requirements.txt

Tested successfully with xAI/Grok - ~$0.007 per explanation

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/business_plan/MatchForge_Analysis_Verified.xlsx
+++ b/business_plan/MatchForge_Analysis_Verified.xlsx
@@ -15,6 +15,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Costs Summary" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ATS History" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ATS Competitors" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AI Roadmap" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3077,4 +3078,423 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>AI ENHANCEMENT ROADMAP (Grok-verified Jan 2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TIER 1: QUICK WINS (1-2 weeks)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Impact</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Cost/1K users</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>LLM Resume Parsing</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>GPT-4/Claude</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Better profile extraction</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>$2-5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>LLM Job Analysis</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>GPT-4/Claude</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>True requirements extraction</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>$2-5</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Natural Language Explanations</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>GPT-4o-mini</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Plain English match reasons</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>$5-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>TIER 2: COMPETITIVE ADVANTAGES (1-2 months)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Impact</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Cost/1K users</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Career Path Prediction</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>LLM + labor data</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Strategic career guidance</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>$5-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Skill Gap Analysis</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>LLM analysis</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Actionable improvement steps</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>$3-5</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Personalized Weights</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Reinforcement learning</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Self-improving algorithm</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>$0 (compute)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>LLM Coach Assistant</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Claude Haiku</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Scale coaching 10x</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>$10-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>TIER 3: MOONSHOTS (3-6 months)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Impact</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Cost/1K users</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Interview Simulation</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>LLM + speech</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Premium coaching feature</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>$20-50</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Bias Detection</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>AI Fairness 360</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Compliance, trust</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>$5-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Market Intelligence</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Real-time APIs</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Strategic positioning</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>$10-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>TOTAL AI COST PROJECTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Tier 1 (MVP+)</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>$9-20/1K users/month</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Tier 1+2 (Growth)</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>$17-35/1K users/month</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Full Stack</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>$50-100/1K users/month</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>ROI AT $19/USER AVG</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Revenue per 1K users</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>$19,000/month</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>AI cost (Tier 1+2)</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>$35/month</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>AI as % of revenue</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>0.18%</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>